<commit_message>
Updated Chidamber and Kemerer Metrics
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 2/team_member_56773/data_collected_metrics.xlsx
+++ b/Project/Phase 1/Sprint 2/team_member_56773/data_collected_metrics.xlsx
@@ -8,13 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GonVirginia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF7D23B-6596-4207-8028-9EFF72FCEB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B448ED-EA7D-4FA9-AC75-81C18DE88421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet3!$B$2:$B$1971</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet3!$B$2:$B$1971</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet3!$G$2:$G$1971</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet3!$C$2:$C$1971</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet3!$G$2:$G$1971</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet3!$G$2:$G$1971</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet3!$C$2:$C$1971</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet3!$E$2:$E$1971</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet3!$D$2:$D$1971</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet3!$G$2:$G$1971</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet3!$F$2:$F$1971</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -6123,6 +6136,4180 @@
 </MapInfo>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>CBO</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>CBO</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{10E10679-1E2C-4D38-9DAC-A64B28FD6277}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>DIT</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>DIT</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{40E91E84-F641-4D0A-96D6-6F276935FC84}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>LCOM</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>LCOM</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{F3C58220-6A8F-4BB5-BF6B-FCBA03C60DD5}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>NOC</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>NOC</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{24AF2D32-EB93-4186-A622-B4689E5E9FF6}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>RFC</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>RFC</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{6C1BA7C7-CAF1-4B98-BB90-3D60B3F4AD14}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.4</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>WMC</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>WMC</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{4EE8BF7B-1CE9-4FE0-BF7B-21541F81B729}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90485</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7461D210-625D-41DB-9615-BEAEDF17B645}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9210675" y="471485"/>
+              <a:ext cx="4610100" cy="7367589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-PT" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F269BB30-BB58-4F28-8BAA-6A4BCCCB3DB1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14106525" y="481013"/>
+              <a:ext cx="2105025" cy="3443288"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-PT" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39D650AE-5E86-4DF9-876E-165F960AE3CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14097001" y="4157661"/>
+              <a:ext cx="4791073" cy="7539039"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-PT" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>100010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F00DF9DA-C90F-4733-A3AB-660814B0E03C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16492537" y="481010"/>
+              <a:ext cx="2786063" cy="3452815"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-PT" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Chart 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA986B99-4200-4169-AB00-60541EB0D374}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9272587" y="12168186"/>
+              <a:ext cx="2900363" cy="5872163"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-PT" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Chart 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A09555C2-4E13-4CB5-930A-65650786EC8F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12482512" y="12206286"/>
+              <a:ext cx="4243388" cy="5376864"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-PT" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5BD7EDEF-2664-4A03-A9E7-B23C4B05F5AD}" name="Table4" displayName="Table4" ref="A1:G1973" totalsRowCount="1" dataDxfId="14" headerRowCellStyle="Accent1">
   <autoFilter ref="A1:G1972" xr:uid="{5BD7EDEF-2664-4A03-A9E7-B23C4B05F5AD}"/>
@@ -6130,23 +10317,23 @@
     <sortCondition descending="1" ref="G1:G1972"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{408301C2-8AE8-4E23-9CEB-70B9C5DACD55}" name="Class" totalsRowLabel="Average" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{9345B7A2-0E61-409A-A126-92DFBE30C625}" name="CBO" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{408301C2-8AE8-4E23-9CEB-70B9C5DACD55}" name="Class" totalsRowLabel="Average" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{9345B7A2-0E61-409A-A126-92DFBE30C625}" name="CBO" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="5">
       <totalsRowFormula>SUBTOTAL(101,B2:B1971)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6753CD0F-9342-44C3-B36A-356DEA7B3B02}" name="DIT" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="3" xr3:uid="{6753CD0F-9342-44C3-B36A-356DEA7B3B02}" name="DIT" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="4">
       <totalsRowFormula>SUBTOTAL(101,C2:C1971)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{72AA4FE8-B1FB-4643-B3D4-AE805ABC21EE}" name="LCOM" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{72AA4FE8-B1FB-4643-B3D4-AE805ABC21EE}" name="LCOM" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="3">
       <totalsRowFormula>SUBTOTAL(101,D2:D1971)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{61B34E37-8DC9-46A0-B5B9-814A02049751}" name="NOC" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{61B34E37-8DC9-46A0-B5B9-814A02049751}" name="NOC" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="2">
       <totalsRowFormula>SUBTOTAL(101,E2:E1971)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1182441A-6260-4D8E-8F63-0B7231D40B0A}" name="RFC" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="6" xr3:uid="{1182441A-6260-4D8E-8F63-0B7231D40B0A}" name="RFC" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="1">
       <totalsRowFormula>SUBTOTAL(101,F2:F1971)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{839EB1E4-D552-41E6-94BC-33E59C61C0BB}" name="WMC" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{839EB1E4-D552-41E6-94BC-33E59C61C0BB}" name="WMC" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="0">
       <totalsRowFormula>SUBTOTAL(101,G2:G1971)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -6453,8 +10640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02917FA-5775-44E2-B485-03102A8741B9}">
   <dimension ref="A1:G1973"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G174" sqref="G2:G174"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50652,8 +54839,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>